<commit_message>
ScriptOverzicht Ingepland + Charachter Controller Update
</commit_message>
<xml_diff>
--- a/Algemeen/ScriptingOverzicht.xlsx
+++ b/Algemeen/ScriptingOverzicht.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>Main Charachter</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>Tutorial/IntroScene</t>
+  </si>
+  <si>
+    <t>Sven</t>
+  </si>
+  <si>
+    <t>Danial</t>
+  </si>
+  <si>
+    <t>Harrold</t>
   </si>
 </sst>
 </file>
@@ -277,12 +286,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -413,23 +446,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -710,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,18 +771,19 @@
     <col min="9" max="9" width="29.5703125" customWidth="1"/>
     <col min="10" max="10" width="34.5703125" customWidth="1"/>
     <col min="11" max="11" width="61" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -768,204 +813,213 @@
       <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="22" t="s">
         <v>20</v>
       </c>
       <c r="K4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="20" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="24" t="s">
         <v>28</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="10" t="s">
         <v>75</v>
       </c>
       <c r="K5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="M5" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="10" t="s">
         <v>76</v>
       </c>
       <c r="K6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="12" t="s">
         <v>38</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="10" t="s">
         <v>77</v>
       </c>
       <c r="K7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="17" t="s">
         <v>70</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="10" t="s">
         <v>79</v>
       </c>
       <c r="K8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="17" t="s">
         <v>60</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="17" t="s">
         <v>71</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="10" t="s">
         <v>80</v>
       </c>
       <c r="K9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>49</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="17" t="s">
         <v>72</v>
       </c>
       <c r="I10" s="13" t="s">
@@ -975,36 +1029,36 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>61</v>
       </c>
       <c r="K11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>52</v>
       </c>
       <c r="K12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>54</v>
       </c>
       <c r="K13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
         <v>49</v>
       </c>
@@ -1030,21 +1084,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F01AFDE7960EE449B48ED2B5A814F5B1" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18441efb09ac3a3cf5f098224069a22d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ec0427ded671ee0047bac0380a5b05">
     <xsd:element name="properties">
@@ -1158,10 +1197,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D050470-434A-4AA6-A444-07B9F70B6F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B12D870-8DBD-4702-8229-A1E1E2E78E4A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1182,17 +1244,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B12D870-8DBD-4702-8229-A1E1E2E78E4A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D050470-434A-4AA6-A444-07B9F70B6F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>